<commit_message>
T2, T5, T6, T7 and T8 commented
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1338,52 +1338,52 @@
         </is>
       </c>
       <c r="B8" s="16" t="n">
-        <v>0.8472475247524753</v>
+        <v>0.8459207920792079</v>
       </c>
       <c r="C8" s="17" t="n">
-        <v>0.04103975245507339</v>
+        <v>0.04455585182996977</v>
       </c>
       <c r="D8" s="17" t="n">
-        <v>0.8132733397566779</v>
+        <v>0.8059709104855858</v>
       </c>
       <c r="E8" s="17" t="n">
-        <v>0.04638460231888916</v>
+        <v>0.04603503786206437</v>
       </c>
       <c r="F8" s="17" t="n">
-        <v>0.9059346405228759</v>
+        <v>0.9152418300653596</v>
       </c>
       <c r="G8" s="17" t="n">
-        <v>0.06453522619906697</v>
+        <v>0.07165552846278239</v>
       </c>
       <c r="H8" s="17" t="n">
-        <v>0.8553851741885583</v>
+        <v>0.8553178420801515</v>
       </c>
       <c r="I8" s="18" t="n">
-        <v>0.03952867817965954</v>
+        <v>0.04329404046302684</v>
       </c>
       <c r="J8" s="16" t="n">
-        <v>0.7678679867986801</v>
+        <v>0.767881188118812</v>
       </c>
       <c r="K8" s="17" t="n">
-        <v>0.04202085438140291</v>
+        <v>0.04230384303784946</v>
       </c>
       <c r="L8" s="17" t="n">
-        <v>0.7453415773017772</v>
+        <v>0.7440600604448825</v>
       </c>
       <c r="M8" s="17" t="n">
-        <v>0.06521820935306404</v>
+        <v>0.06677733342194654</v>
       </c>
       <c r="N8" s="17" t="n">
-        <v>0.8399477124183006</v>
+        <v>0.8425620915032679</v>
       </c>
       <c r="O8" s="17" t="n">
-        <v>0.130626178841875</v>
+        <v>0.1258679662470351</v>
       </c>
       <c r="P8" s="17" t="n">
-        <v>0.7793309524614824</v>
+        <v>0.7803789327126243</v>
       </c>
       <c r="Q8" s="18" t="n">
-        <v>0.05474830280659281</v>
+        <v>0.0529641708465006</v>
       </c>
     </row>
     <row r="9" ht="20.25" customHeight="1">
@@ -1393,52 +1393,52 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>0.9292409240924092</v>
+        <v>0.9253069306930695</v>
       </c>
       <c r="C9" s="8" t="n">
-        <v>0.02308873717261182</v>
+        <v>0.02696885764030971</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>0.8877650338467463</v>
+        <v>0.880477462780817</v>
       </c>
       <c r="E9" s="8" t="n">
-        <v>0.03719288027004294</v>
+        <v>0.03885462910133234</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>0.9854117647058824</v>
+        <v>0.9868496732026144</v>
       </c>
       <c r="G9" s="8" t="n">
-        <v>0.02572947522139783</v>
+        <v>0.02550240699645172</v>
       </c>
       <c r="H9" s="8" t="n">
-        <v>0.9332794644216487</v>
+        <v>0.9300022840041442</v>
       </c>
       <c r="I9" s="9" t="n">
-        <v>0.02030616448194417</v>
+        <v>0.02440057492884872</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>0.8710825082508251</v>
+        <v>0.8823762376237624</v>
       </c>
       <c r="K9" s="8" t="n">
-        <v>0.0273652922256483</v>
+        <v>0.03841772987091333</v>
       </c>
       <c r="L9" s="8" t="n">
-        <v>0.8236576803367675</v>
+        <v>0.8298394374351592</v>
       </c>
       <c r="M9" s="8" t="n">
-        <v>0.02781426747640185</v>
+        <v>0.0417845885789845</v>
       </c>
       <c r="N9" s="8" t="n">
-        <v>0.9456732026143791</v>
+        <v>0.9644183006535948</v>
       </c>
       <c r="O9" s="8" t="n">
-        <v>0.05024014949859574</v>
+        <v>0.03396886397771902</v>
       </c>
       <c r="P9" s="8" t="n">
-        <v>0.8796054059936246</v>
+        <v>0.891670847266695</v>
       </c>
       <c r="Q9" s="9" t="n">
-        <v>0.02752277074878732</v>
+        <v>0.03423675554348856</v>
       </c>
     </row>
     <row r="10" ht="20.25" customHeight="1">

</xml_diff>